<commit_message>
Import/export des resultats/reponses/synthese dans l'autodiag : A BIEN TESTER
</commit_message>
<xml_diff>
--- a/files/autodiag/Gabarit_autodiag.xlsx
+++ b/files/autodiag/Gabarit_autodiag.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-31460" yWindow="1740" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="-35260" yWindow="4800" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="categorie" sheetId="2" r:id="rId1"/>
@@ -12,6 +12,9 @@
     <sheet name="questions" sheetId="3" r:id="rId3"/>
     <sheet name="types" sheetId="4" state="hidden" r:id="rId4"/>
     <sheet name="bool" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="resultats" sheetId="7" r:id="rId6"/>
+    <sheet name="reponses" sheetId="6" r:id="rId7"/>
+    <sheet name="syntheses" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Liste déroulante</t>
   </si>
@@ -107,6 +110,72 @@
   </si>
   <si>
     <t>description_lien_chapitre</t>
+  </si>
+  <si>
+    <t>id_categorie</t>
+  </si>
+  <si>
+    <t>id_chapitre</t>
+  </si>
+  <si>
+    <t>id_question</t>
+  </si>
+  <si>
+    <t>id_reponse</t>
+  </si>
+  <si>
+    <t>valeur_reponse</t>
+  </si>
+  <si>
+    <t>remarque_reponse</t>
+  </si>
+  <si>
+    <t>resultat_reponse</t>
+  </si>
+  <si>
+    <t>question_reponse</t>
+  </si>
+  <si>
+    <t>id_resultat</t>
+  </si>
+  <si>
+    <t>nom_resultat</t>
+  </si>
+  <si>
+    <t>date_derniere_sauvegarde_resultat</t>
+  </si>
+  <si>
+    <t>date_validation_resultat</t>
+  </si>
+  <si>
+    <t>date_creation_resultat</t>
+  </si>
+  <si>
+    <t>taux_remplissage_resultat</t>
+  </si>
+  <si>
+    <t>pdf_resultat</t>
+  </si>
+  <si>
+    <t>remarque_resultat</t>
+  </si>
+  <si>
+    <t>statut_resultat</t>
+  </si>
+  <si>
+    <t>outil_resultat</t>
+  </si>
+  <si>
+    <t>user_resultat</t>
+  </si>
+  <si>
+    <t>synthese_resultat</t>
+  </si>
+  <si>
+    <t>synthese_id</t>
+  </si>
+  <si>
+    <t>resultat_id</t>
   </si>
 </sst>
 </file>
@@ -168,8 +237,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -237,7 +318,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="69">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -266,6 +347,12 @@
     <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -294,6 +381,12 @@
     <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,30 +716,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="18">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
@@ -662,75 +759,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="18">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H1048576">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>0</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>$A$2:$A$985</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>$B$2:$B$985</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -741,96 +841,99 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="27" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="27" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="18">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576 M2:M1048576 G2:G1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 N2:N1048576 H2:H1048576">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>0</formula1>
       <formula2>512</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -838,25 +941,25 @@
           <x14:formula1>
             <xm:f>bool!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>chapitres!$A$2:$A$985</xm:f>
+            <xm:f>chapitres!$B$2:$B$985</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>categorie!$A$2:$A$965</xm:f>
+            <xm:f>categorie!$B$2:$B$965</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>types!A:A</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -930,4 +1033,153 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="23" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#2017 Autodiag : pb lors du changement de code de chapitre
</commit_message>
<xml_diff>
--- a/files/autodiag/Gabarit_autodiag.xlsx
+++ b/files/autodiag/Gabarit_autodiag.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="484" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="484" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="categorie" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>id_categorie</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>numero_chapitre</t>
+  </si>
+  <si>
+    <t>id_chapitre_parent</t>
   </si>
   <si>
     <t>numero_chapitre_parent</t>
@@ -263,18 +266,10 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -292,10 +287,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -322,19 +313,19 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.4555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.8592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="28.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.8333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="4" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -354,61 +345,64 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="21.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="29.0777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="24.6740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="19.8592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="25.3925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.1555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="29.2814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="25.1851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="30"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="3" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="29.0777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.6740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.8592592592593"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.3925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.1555555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.2814814814815"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.1851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="30"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="10.8333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="4" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -437,75 +431,75 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9222222222222"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.537037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="20.1666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="21.0888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="24.7740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="19.2444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="19.6592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="21.6037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="28.8703703703704"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="24.4666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="19.962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="18.737037037037"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="20.062962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="26.1074074074074"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="18.9407407407407"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="17.6074074074074"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="30.5074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="3" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.1666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.0888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.7740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.2444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.6592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.6037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.8703703703704"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.4666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.737037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.062962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="26.1074074074074"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.9407407407407"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.6074074074074"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="30.5074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="10.8333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" s="4" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -537,17 +531,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -613,57 +607,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="14.4296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="18.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="42.5962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="28.6666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="26.4111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="32.1481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="16.5888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="22.5259259259259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="18.737037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.6851851851852"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="21.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="7" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.1481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.737037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.8333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" s="3" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>42</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -684,36 +678,35 @@
   </sheetPr>
   <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="14.162962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="19.6592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="23.6481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="21.1925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="21.8074074074074"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="7" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.162962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.8333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" s="3" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -741,17 +734,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.9925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="21.662962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.662962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.8333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" s="3" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#2456 Autodiag : perte de paramètre lors de l'import
</commit_message>
<xml_diff>
--- a/files/autodiag/Gabarit_autodiag.xlsx
+++ b/files/autodiag/Gabarit_autodiag.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="484" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="484" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="categorie" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,13 +16,15 @@
     <sheet name="resultats" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="reponses" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="syntheses" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="process" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="process_chapitre" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>id_categorie</t>
   </si>
@@ -175,6 +177,21 @@
   </si>
   <si>
     <t>resultat_id</t>
+  </si>
+  <si>
+    <t>process_id</t>
+  </si>
+  <si>
+    <t>process_libelle</t>
+  </si>
+  <si>
+    <t>process_ordre</t>
+  </si>
+  <si>
+    <t>chapitre_id</t>
+  </si>
+  <si>
+    <t>process_chapitre_ordre</t>
   </si>
 </sst>
 </file>
@@ -340,6 +357,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.537037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -347,7 +405,7 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +787,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,4 +814,45 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#2550 export autodiag champs manquants
</commit_message>
<xml_diff>
--- a/files/autodiag/Gabarit_autodiag.xlsx
+++ b/files/autodiag/Gabarit_autodiag.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="484" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="484" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="categorie" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>id_categorie</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>description_lien_chapitre</t>
+  </si>
+  <si>
+    <t>affichage_restitution_barre_chapitre</t>
+  </si>
+  <si>
+    <t>affichage_restitution_radar_chapitre</t>
   </si>
   <si>
     <t>id_question</t>
@@ -364,7 +370,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -378,13 +384,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -403,10 +409,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -422,7 +428,9 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.1851851851852"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.0703703703704"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="30"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.4111111111111"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="42.5962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="10.8333333333333"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,6 +469,12 @@
       </c>
       <c r="L1" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +523,7 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -518,46 +532,46 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -589,17 +603,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -682,40 +696,40 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -752,19 +766,19 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -799,10 +813,10 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -837,13 +851,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>